<commit_message>
added webtable handle concept and javascript executor concept
</commit_message>
<xml_diff>
--- a/bin/com/testdata/NewToursRegTestData.xlsx
+++ b/bin/com/testdata/NewToursRegTestData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11055" windowHeight="5955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11355" windowHeight="5955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="TableData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:H17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>FirstName</t>
   </si>
@@ -148,7 +149,46 @@
     <t>New Delhi</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Alfreds Futterkiste</t>
+  </si>
+  <si>
+    <t>Maria Anders</t>
+  </si>
+  <si>
+    <t>Centro comercial Moctezuma</t>
+  </si>
+  <si>
+    <t>Francisco Chang</t>
+  </si>
+  <si>
+    <t>Ernst Handel</t>
+  </si>
+  <si>
+    <t>Roland Mendel</t>
+  </si>
+  <si>
+    <t>Island Trading</t>
+  </si>
+  <si>
+    <t>Helen Bennett</t>
+  </si>
+  <si>
+    <t>Laughing Bacchus Winecellars</t>
+  </si>
+  <si>
+    <t>Yoshi Tannamuri</t>
+  </si>
+  <si>
+    <t>Magazzini Alimentari Riuniti</t>
+  </si>
+  <si>
+    <t>Giovanni Rovelli</t>
   </si>
 </sst>
 </file>
@@ -207,12 +247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -496,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,11 +548,9 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="14" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -544,14 +581,8 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -583,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -615,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -647,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -679,7 +710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -722,4 +753,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added dropdown helper class
</commit_message>
<xml_diff>
--- a/bin/com/testdata/NewToursRegTestData.xlsx
+++ b/bin/com/testdata/NewToursRegTestData.xlsx
@@ -4,16 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="TableData" sheetId="2" r:id="rId2"/>
+    <sheet name="TableData" r:id="rId5" sheetId="2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -195,6 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,7 +234,12 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
+        <fgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGrid">
         <fgColor indexed="11"/>
       </patternFill>
     </fill>
@@ -257,8 +262,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,17 +547,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -761,28 +766,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.765625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.96484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s" s="5">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -790,7 +793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -798,7 +801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -806,7 +809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -814,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -822,7 +825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -831,6 +834,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added webtable handle code
</commit_message>
<xml_diff>
--- a/bin/com/testdata/NewToursRegTestData.xlsx
+++ b/bin/com/testdata/NewToursRegTestData.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="TableData" r:id="rId5" sheetId="2"/>
+    <sheet name="Table_WorkingExample" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M17"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>FirstName</t>
   </si>
@@ -148,53 +149,25 @@
     <t>New Delhi</t>
   </si>
   <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Contact Name</t>
-  </si>
-  <si>
-    <t>Alfreds Futterkiste</t>
-  </si>
-  <si>
-    <t>Maria Anders</t>
-  </si>
-  <si>
-    <t>Centro comercial Moctezuma</t>
-  </si>
-  <si>
-    <t>Francisco Chang</t>
-  </si>
-  <si>
-    <t>Ernst Handel</t>
-  </si>
-  <si>
-    <t>Roland Mendel</t>
-  </si>
-  <si>
-    <t>Island Trading</t>
-  </si>
-  <si>
-    <t>Helen Bennett</t>
-  </si>
-  <si>
-    <t>Laughing Bacchus Winecellars</t>
-  </si>
-  <si>
-    <t>Yoshi Tannamuri</t>
-  </si>
-  <si>
-    <t>Magazzini Alimentari Riuniti</t>
-  </si>
-  <si>
-    <t>Giovanni Rovelli</t>
+    <t>Gecko</t>
+  </si>
+  <si>
+    <t>Firefox 1.0</t>
+  </si>
+  <si>
+    <t>Win 98+ / OSX.2+</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,12 +207,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightGrid">
+      <patternFill patternType="solid">
         <fgColor indexed="11"/>
       </patternFill>
     </fill>
@@ -257,13 +225,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,17 +518,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -766,74 +737,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.765625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.96484375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s" s="5">
+      <c r="B1" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D1" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="E1" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>